<commit_message>
Multiple choice interest select
</commit_message>
<xml_diff>
--- a/ga.xlsx
+++ b/ga.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="109">
   <si>
     <t>SN</t>
   </si>
@@ -78,175 +78,178 @@
     <t>Yes</t>
   </si>
   <si>
+    <t>Museum, City Experience</t>
+  </si>
+  <si>
+    <t>City Experience</t>
+  </si>
+  <si>
+    <t>Künstler-Nekropole</t>
+  </si>
+  <si>
+    <t>Habichtswald, 34128 Kassel</t>
+  </si>
+  <si>
+    <t>Well-known artists erect their own tombs around the Blue Lake during their lifetime and will also be buried there.</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Cultural Monument</t>
+  </si>
+  <si>
+    <t>Nature</t>
+  </si>
+  <si>
+    <t>Braumanufaktur Steckenpferd</t>
+  </si>
+  <si>
+    <t>Kastenalsgasse 8, 34117 Kassel</t>
+  </si>
+  <si>
+    <t>"Culture meets cuisine" is the motto of the cultural part of our company. The hobby horse should provide space for exhibitions and the presentation of a wide variety of cultural points of view. Whether it’s an exhibition, pop‐up event, lecture or festival. We find the right place in the hobby horse.</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>4,5</t>
+  </si>
+  <si>
+    <t>Eat and Drink</t>
+  </si>
+  <si>
+    <t>denkMAHL Restaurant</t>
+  </si>
+  <si>
+    <t>Friedrich-Ebert-Straße 98, 34119 Kassel</t>
+  </si>
+  <si>
+    <t>Mediterranean-influenced regional dishes at a cozy restaurant with a leafy courtyard.</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>Die Pause</t>
+  </si>
+  <si>
+    <t>Wettergasse 16, 35037 Marburg</t>
+  </si>
+  <si>
+    <t>Dine-In and Takeaway. A little bit hidden on the slope, starting from the Wettergasse.</t>
+  </si>
+  <si>
+    <t>Kaiser-Wilhelm-Turm</t>
+  </si>
+  <si>
+    <t>Hermann-Bauer-Weg 2, 35043 Marburg</t>
+  </si>
+  <si>
+    <t>The Kaiser Wilhelm Tower is a lookout tower on the Lahnberge mountains near Marburg in the Marburg-Biedenkopf district of Hesse. It was built from 1887 to 1890, is 36 m high and has 167 steps inside.</t>
+  </si>
+  <si>
+    <t>Historical Monument</t>
+  </si>
+  <si>
+    <t>History</t>
+  </si>
+  <si>
+    <t>Kurhaus Wiesbaden</t>
+  </si>
+  <si>
+    <t>Kurhauspl. 1, 65189 Wiesbaden</t>
+  </si>
+  <si>
+    <t>The Kurhaus in the Hessian state capital of Wiesbaden is one of the most magnificent permanent buildings in Germany. It is the social center of the spa town of Wiesbaden and offers a representative setting for numerous events.</t>
+  </si>
+  <si>
+    <t>3,4</t>
+  </si>
+  <si>
+    <t>Special Event</t>
+  </si>
+  <si>
+    <t>Henkell &amp; Co. Sektkellerei</t>
+  </si>
+  <si>
+    <t>Biebricher Allee 142, 65187 Wiesbaden</t>
+  </si>
+  <si>
+    <t>Wine Cellar</t>
+  </si>
+  <si>
+    <t>Curry Manufaktur</t>
+  </si>
+  <si>
+    <t>Am Römertor 3, 65183 Wiesbaden</t>
+  </si>
+  <si>
+    <t>Here you can find the menu of Curry Manufaktur . There are currently 22 dishes and drinks on the menu.</t>
+  </si>
+  <si>
+    <t>Kleinmarkthalle</t>
+  </si>
+  <si>
+    <t>Hasengasse 5-7, 60311 Frankfurt am Main</t>
+  </si>
+  <si>
+    <t>Market hall with 60+ vendors selling a variety of groceries, plus flowers, wine &amp; prepared foods.</t>
+  </si>
+  <si>
+    <t>0,4</t>
+  </si>
+  <si>
+    <t>Palmengarten Frankfurt</t>
+  </si>
+  <si>
+    <t>Palmengarten der Stadt, Siesmayerstraße 63, 60323 Frankfurt am Main</t>
+  </si>
+  <si>
+    <t>The Palmengarten is one of three botanical gardens in Frankfurt am Main and is located in the Westend district. With 22 hectares it is one of the largest gardens of its kind in Germany.</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>Schirn Kunsthalle Frankfurt</t>
+  </si>
+  <si>
+    <t>Römerberg, 60311 Frankfurt am Main</t>
+  </si>
+  <si>
+    <t>The Schirn Kunsthalle in the old town of Frankfurt am Main, colloquially simply The Schirn, is one of the well-known exhibition venues in Europe. The Schirn was opened in 1986 and has hosted over 200 exhibitions since then.</t>
+  </si>
+  <si>
+    <t>0,6</t>
+  </si>
+  <si>
+    <t>Art and Culture</t>
+  </si>
+  <si>
+    <t>Obendrüber vom Henschel</t>
+  </si>
+  <si>
+    <t>Marktpl. 2, 64283 Darmstadt</t>
+  </si>
+  <si>
+    <t>The Obendrüber is a modern service restaurant on the roof of the Darmstadt fashion house Henschel. In the evening, after the shop has closed, it can be accessed through a separate entrance on the market square. The menu offers modern, sophisticated crossover cuisine with changing lunch and sophisticated evening dishes</t>
+  </si>
+  <si>
+    <t>Hessisches Landesmuseum Darmstadt</t>
+  </si>
+  <si>
+    <t>Friedenspl. 1, 64283 Darmstadt</t>
+  </si>
+  <si>
+    <t>The Hessian State Museum in Darmstadt, one of the oldest public museums in Germany, is a universal museum with extensive permanent collections; there are also special exhibitions.</t>
+  </si>
+  <si>
     <t>Museum</t>
-  </si>
-  <si>
-    <t>City Experience</t>
-  </si>
-  <si>
-    <t>Künstler-Nekropole</t>
-  </si>
-  <si>
-    <t>Habichtswald, 34128 Kassel</t>
-  </si>
-  <si>
-    <t>Well-known artists erect their own tombs around the Blue Lake during their lifetime and will also be buried there.</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Cultural Monument</t>
-  </si>
-  <si>
-    <t>Nature</t>
-  </si>
-  <si>
-    <t>Braumanufaktur Steckenpferd</t>
-  </si>
-  <si>
-    <t>Kastenalsgasse 8, 34117 Kassel</t>
-  </si>
-  <si>
-    <t>"Culture meets cuisine" is the motto of the cultural part of our company. The hobby horse should provide space for exhibitions and the presentation of a wide variety of cultural points of view. Whether it’s an exhibition, pop‐up event, lecture or festival. We find the right place in the hobby horse.</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>4,5</t>
-  </si>
-  <si>
-    <t>Eat and Drink</t>
-  </si>
-  <si>
-    <t>denkMAHL Restaurant</t>
-  </si>
-  <si>
-    <t>Friedrich-Ebert-Straße 98, 34119 Kassel</t>
-  </si>
-  <si>
-    <t>Mediterranean-influenced regional dishes at a cozy restaurant with a leafy courtyard.</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>Die Pause</t>
-  </si>
-  <si>
-    <t>Wettergasse 16, 35037 Marburg</t>
-  </si>
-  <si>
-    <t>Dine-In and Takeaway. A little bit hidden on the slope, starting from the Wettergasse.</t>
-  </si>
-  <si>
-    <t>Kaiser-Wilhelm-Turm</t>
-  </si>
-  <si>
-    <t>Hermann-Bauer-Weg 2, 35043 Marburg</t>
-  </si>
-  <si>
-    <t>The Kaiser Wilhelm Tower is a lookout tower on the Lahnberge mountains near Marburg in the Marburg-Biedenkopf district of Hesse. It was built from 1887 to 1890, is 36 m high and has 167 steps inside.</t>
-  </si>
-  <si>
-    <t>Historical Monument</t>
-  </si>
-  <si>
-    <t>History</t>
-  </si>
-  <si>
-    <t>Kurhaus Wiesbaden</t>
-  </si>
-  <si>
-    <t>Kurhauspl. 1, 65189 Wiesbaden</t>
-  </si>
-  <si>
-    <t>The Kurhaus in the Hessian state capital of Wiesbaden is one of the most magnificent permanent buildings in Germany. It is the social center of the spa town of Wiesbaden and offers a representative setting for numerous events.</t>
-  </si>
-  <si>
-    <t>3,4</t>
-  </si>
-  <si>
-    <t>Special Event</t>
-  </si>
-  <si>
-    <t>Henkell &amp; Co. Sektkellerei</t>
-  </si>
-  <si>
-    <t>Biebricher Allee 142, 65187 Wiesbaden</t>
-  </si>
-  <si>
-    <t>Wine Cellar</t>
-  </si>
-  <si>
-    <t>Curry Manufaktur</t>
-  </si>
-  <si>
-    <t>Am Römertor 3, 65183 Wiesbaden</t>
-  </si>
-  <si>
-    <t>Here you can find the menu of Curry Manufaktur . There are currently 22 dishes and drinks on the menu.</t>
-  </si>
-  <si>
-    <t>Kleinmarkthalle</t>
-  </si>
-  <si>
-    <t>Hasengasse 5-7, 60311 Frankfurt am Main</t>
-  </si>
-  <si>
-    <t>Market hall with 60+ vendors selling a variety of groceries, plus flowers, wine &amp; prepared foods.</t>
-  </si>
-  <si>
-    <t>0,4</t>
-  </si>
-  <si>
-    <t>Palmengarten Frankfurt</t>
-  </si>
-  <si>
-    <t>Palmengarten der Stadt, Siesmayerstraße 63, 60323 Frankfurt am Main</t>
-  </si>
-  <si>
-    <t>The Palmengarten is one of three botanical gardens in Frankfurt am Main and is located in the Westend district. With 22 hectares it is one of the largest gardens of its kind in Germany.</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>Schirn Kunsthalle Frankfurt</t>
-  </si>
-  <si>
-    <t>Römerberg, 60311 Frankfurt am Main</t>
-  </si>
-  <si>
-    <t>The Schirn Kunsthalle in the old town of Frankfurt am Main, colloquially simply The Schirn, is one of the well-known exhibition venues in Europe. The Schirn was opened in 1986 and has hosted over 200 exhibitions since then.</t>
-  </si>
-  <si>
-    <t>0,6</t>
-  </si>
-  <si>
-    <t>Art and Culture</t>
-  </si>
-  <si>
-    <t>Obendrüber vom Henschel</t>
-  </si>
-  <si>
-    <t>Marktpl. 2, 64283 Darmstadt</t>
-  </si>
-  <si>
-    <t>The Obendrüber is a modern service restaurant on the roof of the Darmstadt fashion house Henschel. In the evening, after the shop has closed, it can be accessed through a separate entrance on the market square. The menu offers modern, sophisticated crossover cuisine with changing lunch and sophisticated evening dishes</t>
-  </si>
-  <si>
-    <t>Hessisches Landesmuseum Darmstadt</t>
-  </si>
-  <si>
-    <t>Friedenspl. 1, 64283 Darmstadt</t>
-  </si>
-  <si>
-    <t>The Hessian State Museum in Darmstadt, one of the oldest public museums in Germany, is a universal museum with extensive permanent collections; there are also special exhibitions.</t>
   </si>
   <si>
     <t>Mathildenhöhe Darmstadt</t>
@@ -1398,7 +1401,7 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="15.75" customHeight="1"/>
@@ -1408,6 +1411,7 @@
     <col min="4" max="4" width="29.6339285714286" customWidth="1"/>
     <col min="9" max="9" width="18.3839285714286" customWidth="1"/>
     <col min="10" max="10" width="17.5" customWidth="1"/>
+    <col min="14" max="14" width="47.7589285714286" customWidth="1"/>
     <col min="15" max="15" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2034,7 +2038,7 @@
         <v>19</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>20</v>
+        <v>77</v>
       </c>
       <c r="O15" s="5" t="s">
         <v>46</v>
@@ -2048,10 +2052,10 @@
         <v>1</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E16" s="4">
         <v>49.88</v>
@@ -2060,7 +2064,7 @@
         <v>8.67</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>18</v>
@@ -2085,10 +2089,10 @@
         <v>1</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E17" s="4">
         <v>50.58</v>
@@ -2097,7 +2101,7 @@
         <v>8.67</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H17" s="7" t="s">
         <v>32</v>
@@ -2110,7 +2114,7 @@
         <v>19</v>
       </c>
       <c r="N17" s="5" t="s">
-        <v>20</v>
+        <v>77</v>
       </c>
       <c r="O17" s="5"/>
     </row>
@@ -2122,10 +2126,10 @@
         <v>1</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E18" s="4">
         <v>50.58</v>
@@ -2134,14 +2138,14 @@
         <v>8.67</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>65</v>
       </c>
       <c r="I18" s="17"/>
       <c r="J18" s="13" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K18" s="16">
         <v>11</v>
@@ -2153,7 +2157,7 @@
         <v>19</v>
       </c>
       <c r="N18" s="5" t="s">
-        <v>20</v>
+        <v>77</v>
       </c>
       <c r="O18" s="5"/>
     </row>
@@ -2165,10 +2169,10 @@
         <v>1</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E19" s="4">
         <v>50.59</v>
@@ -2177,7 +2181,7 @@
         <v>8.68</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H19" s="7" t="s">
         <v>65</v>
@@ -2192,7 +2196,7 @@
         <v>19</v>
       </c>
       <c r="N19" s="5" t="s">
-        <v>20</v>
+        <v>77</v>
       </c>
       <c r="O19" s="5"/>
     </row>
@@ -2204,10 +2208,10 @@
         <v>1</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E20" s="4">
         <v>50.56</v>
@@ -2216,7 +2220,7 @@
         <v>8.5</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H20" s="7" t="s">
         <v>38</v>
@@ -2243,10 +2247,10 @@
         <v>1</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E21" s="4">
         <v>50.55</v>
@@ -2255,7 +2259,7 @@
         <v>8.51</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H21" s="7" t="s">
         <v>18</v>
@@ -2286,15 +2290,15 @@
         <v>1</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H22" s="7" t="s">
         <v>32</v>
@@ -2303,15 +2307,19 @@
         <v>10</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
+        <v>100</v>
+      </c>
+      <c r="K22" s="15">
+        <v>10</v>
+      </c>
+      <c r="L22" s="15">
+        <v>15</v>
+      </c>
       <c r="M22" s="5" t="s">
         <v>26</v>
       </c>
       <c r="N22" s="5" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="O22" s="5" t="s">
         <v>46</v>
@@ -2338,42 +2346,42 @@
   <sheetData>
     <row r="2" customHeight="1" spans="2:2">
       <c r="B2" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="2:2">
       <c r="B3" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="2:2">
       <c r="B4" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="2:2">
       <c r="B5" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="2:2">
       <c r="B6" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="2:2">
       <c r="B7" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="2:2">
       <c r="B8" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="2:2">
       <c r="B9" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove additional interest field
</commit_message>
<xml_diff>
--- a/ga.xlsx
+++ b/ga.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="106">
   <si>
     <t>SN</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Interest</t>
   </si>
   <si>
-    <t>Interest additional</t>
-  </si>
-  <si>
     <t>GRIMMWELT Kassel gGmbH</t>
   </si>
   <si>
@@ -81,139 +78,133 @@
     <t>Museum, City Experience</t>
   </si>
   <si>
+    <t>Künstler-Nekropole</t>
+  </si>
+  <si>
+    <t>Habichtswald, 34128 Kassel</t>
+  </si>
+  <si>
+    <t>Well-known artists erect their own tombs around the Blue Lake during their lifetime and will also be buried there.</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Cultural Monument</t>
+  </si>
+  <si>
+    <t>Braumanufaktur Steckenpferd</t>
+  </si>
+  <si>
+    <t>Kastenalsgasse 8, 34117 Kassel</t>
+  </si>
+  <si>
+    <t>"Culture meets cuisine" is the motto of the cultural part of our company. The hobby horse should provide space for exhibitions and the presentation of a wide variety of cultural points of view. Whether it’s an exhibition, pop‐up event, lecture or festival. We find the right place in the hobby horse.</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>4,5</t>
+  </si>
+  <si>
+    <t>Eat and Drink</t>
+  </si>
+  <si>
+    <t>denkMAHL Restaurant</t>
+  </si>
+  <si>
+    <t>Friedrich-Ebert-Straße 98, 34119 Kassel</t>
+  </si>
+  <si>
+    <t>Mediterranean-influenced regional dishes at a cozy restaurant with a leafy courtyard.</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>Die Pause</t>
+  </si>
+  <si>
+    <t>Wettergasse 16, 35037 Marburg</t>
+  </si>
+  <si>
+    <t>Dine-In and Takeaway. A little bit hidden on the slope, starting from the Wettergasse.</t>
+  </si>
+  <si>
+    <t>Kaiser-Wilhelm-Turm</t>
+  </si>
+  <si>
+    <t>Hermann-Bauer-Weg 2, 35043 Marburg</t>
+  </si>
+  <si>
+    <t>The Kaiser Wilhelm Tower is a lookout tower on the Lahnberge mountains near Marburg in the Marburg-Biedenkopf district of Hesse. It was built from 1887 to 1890, is 36 m high and has 167 steps inside.</t>
+  </si>
+  <si>
+    <t>Historical Monument</t>
+  </si>
+  <si>
+    <t>Kurhaus Wiesbaden</t>
+  </si>
+  <si>
+    <t>Kurhauspl. 1, 65189 Wiesbaden</t>
+  </si>
+  <si>
+    <t>The Kurhaus in the Hessian state capital of Wiesbaden is one of the most magnificent permanent buildings in Germany. It is the social center of the spa town of Wiesbaden and offers a representative setting for numerous events.</t>
+  </si>
+  <si>
+    <t>3,4</t>
+  </si>
+  <si>
+    <t>Henkell &amp; Co. Sektkellerei</t>
+  </si>
+  <si>
+    <t>Biebricher Allee 142, 65187 Wiesbaden</t>
+  </si>
+  <si>
+    <t>Wine Cellar</t>
+  </si>
+  <si>
     <t>City Experience</t>
   </si>
   <si>
-    <t>Künstler-Nekropole</t>
-  </si>
-  <si>
-    <t>Habichtswald, 34128 Kassel</t>
-  </si>
-  <si>
-    <t>Well-known artists erect their own tombs around the Blue Lake during their lifetime and will also be buried there.</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Cultural Monument</t>
+    <t>Curry Manufaktur</t>
+  </si>
+  <si>
+    <t>Am Römertor 3, 65183 Wiesbaden</t>
+  </si>
+  <si>
+    <t>Here you can find the menu of Curry Manufaktur . There are currently 22 dishes and drinks on the menu.</t>
+  </si>
+  <si>
+    <t>Kleinmarkthalle</t>
+  </si>
+  <si>
+    <t>Hasengasse 5-7, 60311 Frankfurt am Main</t>
+  </si>
+  <si>
+    <t>Market hall with 60+ vendors selling a variety of groceries, plus flowers, wine &amp; prepared foods.</t>
+  </si>
+  <si>
+    <t>0,4</t>
+  </si>
+  <si>
+    <t>Palmengarten Frankfurt</t>
+  </si>
+  <si>
+    <t>Palmengarten der Stadt, Siesmayerstraße 63, 60323 Frankfurt am Main</t>
+  </si>
+  <si>
+    <t>The Palmengarten is one of three botanical gardens in Frankfurt am Main and is located in the Westend district. With 22 hectares it is one of the largest gardens of its kind in Germany.</t>
+  </si>
+  <si>
+    <t>e</t>
   </si>
   <si>
     <t>Nature</t>
-  </si>
-  <si>
-    <t>Braumanufaktur Steckenpferd</t>
-  </si>
-  <si>
-    <t>Kastenalsgasse 8, 34117 Kassel</t>
-  </si>
-  <si>
-    <t>"Culture meets cuisine" is the motto of the cultural part of our company. The hobby horse should provide space for exhibitions and the presentation of a wide variety of cultural points of view. Whether it’s an exhibition, pop‐up event, lecture or festival. We find the right place in the hobby horse.</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>4,5</t>
-  </si>
-  <si>
-    <t>Eat and Drink</t>
-  </si>
-  <si>
-    <t>denkMAHL Restaurant</t>
-  </si>
-  <si>
-    <t>Friedrich-Ebert-Straße 98, 34119 Kassel</t>
-  </si>
-  <si>
-    <t>Mediterranean-influenced regional dishes at a cozy restaurant with a leafy courtyard.</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>Die Pause</t>
-  </si>
-  <si>
-    <t>Wettergasse 16, 35037 Marburg</t>
-  </si>
-  <si>
-    <t>Dine-In and Takeaway. A little bit hidden on the slope, starting from the Wettergasse.</t>
-  </si>
-  <si>
-    <t>Kaiser-Wilhelm-Turm</t>
-  </si>
-  <si>
-    <t>Hermann-Bauer-Weg 2, 35043 Marburg</t>
-  </si>
-  <si>
-    <t>The Kaiser Wilhelm Tower is a lookout tower on the Lahnberge mountains near Marburg in the Marburg-Biedenkopf district of Hesse. It was built from 1887 to 1890, is 36 m high and has 167 steps inside.</t>
-  </si>
-  <si>
-    <t>Historical Monument</t>
-  </si>
-  <si>
-    <t>History</t>
-  </si>
-  <si>
-    <t>Kurhaus Wiesbaden</t>
-  </si>
-  <si>
-    <t>Kurhauspl. 1, 65189 Wiesbaden</t>
-  </si>
-  <si>
-    <t>The Kurhaus in the Hessian state capital of Wiesbaden is one of the most magnificent permanent buildings in Germany. It is the social center of the spa town of Wiesbaden and offers a representative setting for numerous events.</t>
-  </si>
-  <si>
-    <t>3,4</t>
-  </si>
-  <si>
-    <t>Special Event</t>
-  </si>
-  <si>
-    <t>Henkell &amp; Co. Sektkellerei</t>
-  </si>
-  <si>
-    <t>Biebricher Allee 142, 65187 Wiesbaden</t>
-  </si>
-  <si>
-    <t>Wine Cellar</t>
-  </si>
-  <si>
-    <t>Curry Manufaktur</t>
-  </si>
-  <si>
-    <t>Am Römertor 3, 65183 Wiesbaden</t>
-  </si>
-  <si>
-    <t>Here you can find the menu of Curry Manufaktur . There are currently 22 dishes and drinks on the menu.</t>
-  </si>
-  <si>
-    <t>Kleinmarkthalle</t>
-  </si>
-  <si>
-    <t>Hasengasse 5-7, 60311 Frankfurt am Main</t>
-  </si>
-  <si>
-    <t>Market hall with 60+ vendors selling a variety of groceries, plus flowers, wine &amp; prepared foods.</t>
-  </si>
-  <si>
-    <t>0,4</t>
-  </si>
-  <si>
-    <t>Palmengarten Frankfurt</t>
-  </si>
-  <si>
-    <t>Palmengarten der Stadt, Siesmayerstraße 63, 60323 Frankfurt am Main</t>
-  </si>
-  <si>
-    <t>The Palmengarten is one of three botanical gardens in Frankfurt am Main and is located in the Westend district. With 22 hectares it is one of the largest gardens of its kind in Germany.</t>
-  </si>
-  <si>
-    <t>e</t>
   </si>
   <si>
     <t>Schirn Kunsthalle Frankfurt</t>
@@ -1398,10 +1389,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6339285714286" defaultRowHeight="15.75" customHeight="1"/>
@@ -1412,10 +1403,9 @@
     <col min="9" max="9" width="18.3839285714286" customWidth="1"/>
     <col min="10" max="10" width="17.5" customWidth="1"/>
     <col min="14" max="14" width="47.7589285714286" customWidth="1"/>
-    <col min="15" max="15" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:15">
+    <row r="1" customHeight="1" spans="1:14">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1458,11 +1448,8 @@
       <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" customHeight="1" spans="1:15">
+    </row>
+    <row r="2" customHeight="1" spans="1:14">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1470,10 +1457,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="E2" s="4">
         <v>51.31</v>
@@ -1482,10 +1469,10 @@
         <v>9.49</v>
       </c>
       <c r="G2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>17</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>18</v>
       </c>
       <c r="I2" s="8">
         <v>10</v>
@@ -1498,16 +1485,13 @@
         <v>14</v>
       </c>
       <c r="M2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" customHeight="1" spans="1:15">
+    </row>
+    <row r="3" customHeight="1" spans="1:14">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1515,10 +1499,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E3" s="4">
         <v>51.32</v>
@@ -1527,10 +1511,10 @@
         <v>9.45</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I3" s="12"/>
       <c r="J3" s="13"/>
@@ -1541,16 +1525,13 @@
         <v>17</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" customHeight="1" spans="1:15">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" customHeight="1" spans="1:14">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -1558,10 +1539,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E4" s="4">
         <v>51.32</v>
@@ -1570,30 +1551,27 @@
         <v>9.5</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I4" s="12">
         <v>5</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="K4" s="15"/>
       <c r="L4" s="15"/>
       <c r="M4" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" customHeight="1" spans="1:15">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" customHeight="1" spans="1:14">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1601,10 +1579,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E5" s="4">
         <v>51.32</v>
@@ -1613,10 +1591,10 @@
         <v>9.47</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I5" s="12"/>
       <c r="J5" s="15"/>
@@ -1627,16 +1605,13 @@
         <v>16</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" customHeight="1" spans="1:15">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" customHeight="1" spans="1:14">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -1644,10 +1619,10 @@
         <v>1</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E6" s="4">
         <v>50.81</v>
@@ -1656,10 +1631,10 @@
         <v>8.77</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I6" s="17">
         <v>2</v>
@@ -1668,16 +1643,13 @@
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
       <c r="M6" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" customHeight="1" spans="1:15">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" customHeight="1" spans="1:14">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1685,10 +1657,10 @@
         <v>1</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E7" s="4">
         <v>50.82</v>
@@ -1697,26 +1669,23 @@
         <v>8.79</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I7" s="12"/>
       <c r="J7" s="13"/>
       <c r="K7" s="15"/>
       <c r="L7" s="15"/>
       <c r="M7" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="O7" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" customHeight="1" spans="1:15">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" customHeight="1" spans="1:14">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1724,10 +1693,10 @@
         <v>1</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E8" s="4">
         <v>50.08</v>
@@ -1736,30 +1705,27 @@
         <v>8.25</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I8" s="17">
         <v>8</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K8" s="15"/>
       <c r="L8" s="15"/>
       <c r="M8" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="O8" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" customHeight="1" spans="1:15">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" customHeight="1" spans="1:14">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1767,10 +1733,10 @@
         <v>1</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E9" s="4">
         <v>50.05</v>
@@ -1779,24 +1745,23 @@
         <v>8.24</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I9" s="12"/>
       <c r="J9" s="13"/>
       <c r="K9" s="15"/>
       <c r="L9" s="13"/>
       <c r="M9" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="O9" s="5"/>
-    </row>
-    <row r="10" customHeight="1" spans="1:15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" customHeight="1" spans="1:14">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1804,10 +1769,10 @@
         <v>1</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E10" s="4">
         <v>50.08</v>
@@ -1816,10 +1781,10 @@
         <v>8.24</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I10" s="17"/>
       <c r="J10" s="13"/>
@@ -1830,16 +1795,13 @@
         <v>18</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="O10" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" customHeight="1" spans="1:15">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" customHeight="1" spans="1:14">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -1847,10 +1809,10 @@
         <v>1</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E11" s="4">
         <v>50.11</v>
@@ -1859,28 +1821,27 @@
         <v>8.68</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I11" s="12">
         <v>4</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="K11" s="13"/>
       <c r="L11" s="13"/>
       <c r="M11" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="O11" s="5"/>
-    </row>
-    <row r="12" customHeight="1" spans="1:15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" customHeight="1" spans="1:14">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -1888,10 +1849,10 @@
         <v>1</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E12" s="4">
         <v>50.12</v>
@@ -1900,26 +1861,23 @@
         <v>8.66</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I12" s="17"/>
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
       <c r="M12" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="O12" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" customHeight="1" spans="1:15">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" customHeight="1" spans="1:14">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -1927,10 +1885,10 @@
         <v>1</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E13" s="4">
         <v>50.11</v>
@@ -1939,28 +1897,25 @@
         <v>8.68</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I13" s="17"/>
       <c r="J13" s="13" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
       <c r="M13" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N13" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="O13" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" customHeight="1" spans="1:15">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" customHeight="1" spans="1:14">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -1968,10 +1923,10 @@
         <v>1</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E14" s="4">
         <v>49.87</v>
@@ -1980,26 +1935,23 @@
         <v>8.65</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I14" s="12"/>
       <c r="J14" s="13"/>
       <c r="K14" s="13"/>
       <c r="L14" s="13"/>
       <c r="M14" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N14" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="O14" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" customHeight="1" spans="1:15">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" customHeight="1" spans="1:14">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -2007,10 +1959,10 @@
         <v>1</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E15" s="4">
         <v>49.87</v>
@@ -2019,10 +1971,10 @@
         <v>8.65</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I15" s="17">
         <v>10</v>
@@ -2035,16 +1987,13 @@
         <v>18</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="O15" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" customHeight="1" spans="1:15">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" customHeight="1" spans="1:14">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -2052,10 +2001,10 @@
         <v>1</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E16" s="4">
         <v>49.88</v>
@@ -2064,24 +2013,23 @@
         <v>8.67</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I16" s="17"/>
       <c r="J16" s="13"/>
       <c r="K16" s="13"/>
       <c r="L16" s="13"/>
       <c r="M16" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N16" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="O16" s="5"/>
-    </row>
-    <row r="17" customHeight="1" spans="1:15">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" customHeight="1" spans="1:14">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -2089,10 +2037,10 @@
         <v>1</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E17" s="4">
         <v>50.58</v>
@@ -2101,24 +2049,23 @@
         <v>8.67</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I17" s="17"/>
       <c r="J17" s="13"/>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
       <c r="M17" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N17" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="O17" s="5"/>
-    </row>
-    <row r="18" customHeight="1" spans="1:15">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" customHeight="1" spans="1:14">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -2126,10 +2073,10 @@
         <v>1</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E18" s="4">
         <v>50.58</v>
@@ -2138,14 +2085,14 @@
         <v>8.67</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I18" s="17"/>
       <c r="J18" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="K18" s="16">
         <v>11</v>
@@ -2154,14 +2101,13 @@
         <v>14</v>
       </c>
       <c r="M18" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N18" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="O18" s="5"/>
-    </row>
-    <row r="19" customHeight="1" spans="1:15">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" customHeight="1" spans="1:14">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -2169,10 +2115,10 @@
         <v>1</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E19" s="4">
         <v>50.59</v>
@@ -2181,10 +2127,10 @@
         <v>8.68</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I19" s="12">
         <v>6</v>
@@ -2193,14 +2139,13 @@
       <c r="K19" s="15"/>
       <c r="L19" s="15"/>
       <c r="M19" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N19" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="O19" s="5"/>
-    </row>
-    <row r="20" customHeight="1" spans="1:15">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" customHeight="1" spans="1:14">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -2208,10 +2153,10 @@
         <v>1</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E20" s="4">
         <v>50.56</v>
@@ -2220,26 +2165,23 @@
         <v>8.5</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I20" s="12"/>
       <c r="J20" s="13"/>
       <c r="K20" s="13"/>
       <c r="L20" s="13"/>
       <c r="M20" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N20" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="O20" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" customHeight="1" spans="1:15">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" customHeight="1" spans="1:14">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -2247,10 +2189,10 @@
         <v>1</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E21" s="4">
         <v>50.55</v>
@@ -2259,10 +2201,10 @@
         <v>8.51</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I21" s="12"/>
       <c r="J21" s="13"/>
@@ -2273,16 +2215,13 @@
         <v>18</v>
       </c>
       <c r="M21" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N21" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="O21" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" customHeight="1" spans="1:15">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" customHeight="1" spans="1:14">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -2290,24 +2229,24 @@
         <v>1</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I22" s="12">
         <v>10</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="K22" s="15">
         <v>10</v>
@@ -2316,13 +2255,10 @@
         <v>15</v>
       </c>
       <c r="M22" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N22" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="O22" s="5" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -2346,42 +2282,42 @@
   <sheetData>
     <row r="2" customHeight="1" spans="2:2">
       <c r="B2" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="2:2">
       <c r="B3" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="2:2">
       <c r="B4" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="2:2">
       <c r="B5" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="2:2">
       <c r="B6" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="2:2">
       <c r="B7" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="2:2">
       <c r="B8" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="2:2">
       <c r="B9" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>